<commit_message>
used to execute 01.dat
</commit_message>
<xml_diff>
--- a/01 vl.xlsx
+++ b/01 vl.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12120" windowHeight="7380"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>道路區塊總面積</t>
   </si>
@@ -62,6 +62,57 @@
   </si>
   <si>
     <t>Cost</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Road</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Area</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PCI</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>:011011011</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>:001101011</t>
+  </si>
+  <si>
+    <t>:011111010</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>:111011011</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>:010111110</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>:111011010</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>:011101010</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>:111110010</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>:001101001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>:011111010</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -69,6 +120,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="2">
+    <numFmt numFmtId="176" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="177" formatCode="#,##0.00_);[Red]\(#,##0.00\)"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -99,7 +154,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -107,11 +162,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -124,6 +194,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -405,10 +487,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -416,10 +498,12 @@
     <col min="1" max="1" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
@@ -436,7 +520,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -450,12 +534,22 @@
         <f>(100 - C2*0.8)*B2</f>
         <v>158681.44884751999</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="7">
         <f>B2*586</f>
         <v>1276577.56</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" s="3">
+        <v>0</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" s="8">
+        <f>E5+E4+E7+E10</f>
+        <v>20085296.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -469,12 +563,22 @@
         <f t="shared" ref="D3:D10" si="0">(100 - C3*0.8)*B3</f>
         <v>536138.81374320004</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="7">
         <f t="shared" ref="E3:E10" si="1">B3*586</f>
         <v>7442117.96</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" s="3">
+        <v>1</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="8">
+        <f>E3+E4+E6+E7+E9+E10</f>
+        <v>44265350.039999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -488,12 +592,22 @@
         <f t="shared" si="0"/>
         <v>871241.14638847997</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="7">
         <f t="shared" si="1"/>
         <v>11973040.66</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" s="3">
+        <v>2</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" s="8">
+        <f>E4+E5+E7+E9+E10</f>
+        <v>33093828.460000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -507,12 +621,22 @@
         <f t="shared" si="0"/>
         <v>29626.359070559996</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="7">
         <f t="shared" si="1"/>
         <v>625719.07999999996</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5" s="3">
+        <v>3</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" s="8">
+        <f>E9+E7+E6+E5+E4+E3</f>
+        <v>44049250.82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -526,12 +650,22 @@
         <f t="shared" si="0"/>
         <v>148639</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="7">
         <f t="shared" si="1"/>
         <v>4355122.7</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6" s="3">
+        <v>4</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6" s="8">
+        <f>E9+E7+E6+E5+E4+E3</f>
+        <v>44049250.82</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -545,12 +679,22 @@
         <f t="shared" si="0"/>
         <v>416498.93580623996</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="7">
         <f t="shared" si="1"/>
         <v>6644718.46</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7" s="3">
+        <v>5</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H7" s="8">
+        <f>E2+E3+E4+E6+E7+E9+E10</f>
+        <v>45541927.599999994</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -564,12 +708,22 @@
         <f t="shared" si="0"/>
         <v>492497.4979668</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="7">
         <f t="shared" si="1"/>
         <v>3432547.74</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8" s="3">
+        <v>6</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H8" s="8">
+        <f>E3+E5+E6+E7+E8+E9</f>
+        <v>35508757.899999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -583,12 +737,19 @@
         <f t="shared" si="0"/>
         <v>1780174.7105284799</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="7">
         <f t="shared" si="1"/>
         <v>13008531.960000001</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9" s="3">
+        <v>7</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H9" s="8"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -602,9 +763,91 @@
         <f t="shared" si="0"/>
         <v>130964.3219292</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="7">
         <f t="shared" si="1"/>
         <v>841818.29999999993</v>
+      </c>
+      <c r="F10" s="3">
+        <v>8</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H10" s="8"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F11" s="3">
+        <v>9</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H11" s="8"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="6">
+        <v>1</v>
+      </c>
+      <c r="B13" s="6">
+        <v>2178.46</v>
+      </c>
+      <c r="C13" s="6">
+        <v>33.948610000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="6">
+        <v>2</v>
+      </c>
+      <c r="B14" s="6">
+        <v>12699.86</v>
+      </c>
+      <c r="C14" s="6">
+        <v>72.229849999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="6">
+        <v>3</v>
+      </c>
+      <c r="B15" s="6">
+        <v>20431.810000000001</v>
+      </c>
+      <c r="C15" s="6">
+        <v>71.698239999999998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="6">
+        <v>4</v>
+      </c>
+      <c r="B16" s="6">
+        <v>1067.78</v>
+      </c>
+      <c r="C16" s="6">
+        <v>90.317809999999994</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="6">
+        <v>5</v>
+      </c>
+      <c r="B17" s="6">
+        <v>7431.95</v>
+      </c>
+      <c r="C17" s="6">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>